<commit_message>
Data and code for change detection evaluation
</commit_message>
<xml_diff>
--- a/Well_Validation.xlsx
+++ b/Well_Validation.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2279" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2414" uniqueCount="43">
   <si>
     <t>FID</t>
   </si>
@@ -141,6 +141,21 @@
   </si>
   <si>
     <t>Scrub</t>
+  </si>
+  <si>
+    <t>Cochran</t>
+  </si>
+  <si>
+    <t>cv</t>
+  </si>
+  <si>
+    <t>rcv</t>
+  </si>
+  <si>
+    <t>ndvi</t>
+  </si>
+  <si>
+    <t>ndsi</t>
   </si>
 </sst>
 </file>
@@ -492,11 +507,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M446"/>
+  <dimension ref="A1:V494"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A201" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T382" sqref="T382"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A380" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P393" sqref="P393:S409"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8239,7 +8254,7 @@
         <v>294.61399999999998</v>
       </c>
       <c r="E194">
-        <f t="shared" ref="E194:E257" si="6">D194/C194</f>
+        <f t="shared" ref="E194:E232" si="6">D194/C194</f>
         <v>0.7958662692898375</v>
       </c>
       <c r="F194">
@@ -14585,7 +14600,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="369" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>380</v>
       </c>
@@ -14625,7 +14640,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="370" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>391</v>
       </c>
@@ -14665,7 +14680,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="371" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>394</v>
       </c>
@@ -14705,7 +14720,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="372" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>398</v>
       </c>
@@ -14745,7 +14760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="373" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>408</v>
       </c>
@@ -14785,7 +14800,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="374" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>410</v>
       </c>
@@ -14825,7 +14840,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="375" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>415</v>
       </c>
@@ -14865,7 +14880,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="376" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>440</v>
       </c>
@@ -14905,7 +14920,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="377" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>442</v>
       </c>
@@ -14948,7 +14963,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="378" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>449</v>
       </c>
@@ -14988,7 +15003,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="379" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>462</v>
       </c>
@@ -15028,7 +15043,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="380" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>468</v>
       </c>
@@ -15068,7 +15083,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="381" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>475</v>
       </c>
@@ -15107,8 +15122,20 @@
       <c r="L381" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="382" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="S381">
+        <v>0.75</v>
+      </c>
+      <c r="T381">
+        <v>1</v>
+      </c>
+      <c r="U381">
+        <v>1.5</v>
+      </c>
+      <c r="V381">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="382" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A382">
         <v>480</v>
       </c>
@@ -15147,8 +15174,33 @@
       <c r="L382" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="383" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P382" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q382">
+        <v>6.25</v>
+      </c>
+      <c r="R382">
+        <v>2664786.9</v>
+      </c>
+      <c r="S382">
+        <f>$Q382+($R382*S$381)</f>
+        <v>1998596.4249999998</v>
+      </c>
+      <c r="T382">
+        <f>$Q382+($R382*T$381)</f>
+        <v>2664793.15</v>
+      </c>
+      <c r="U382">
+        <f t="shared" ref="U382:V384" si="14">$Q382+($R382*U$381)</f>
+        <v>3997186.5999999996</v>
+      </c>
+      <c r="V382">
+        <f t="shared" si="14"/>
+        <v>5329580.05</v>
+      </c>
+    </row>
+    <row r="383" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>481</v>
       </c>
@@ -15187,8 +15239,33 @@
       <c r="L383" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="384" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P383" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q383">
+        <v>1.75E-4</v>
+      </c>
+      <c r="R383">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="S383">
+        <f t="shared" ref="S383:T384" si="15">$Q383+($R383*S$381)</f>
+        <v>0.24242500000000003</v>
+      </c>
+      <c r="T383">
+        <f t="shared" si="15"/>
+        <v>0.32317499999999999</v>
+      </c>
+      <c r="U383">
+        <f t="shared" si="14"/>
+        <v>0.48467500000000002</v>
+      </c>
+      <c r="V383">
+        <f t="shared" si="14"/>
+        <v>0.64617500000000005</v>
+      </c>
+    </row>
+    <row r="384" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>494</v>
       </c>
@@ -15227,8 +15304,33 @@
       <c r="L384" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="385" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P384" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q384">
+        <v>4.6464999999999999E-2</v>
+      </c>
+      <c r="R384">
+        <v>0.12520000000000001</v>
+      </c>
+      <c r="S384">
+        <f t="shared" si="15"/>
+        <v>0.14036500000000002</v>
+      </c>
+      <c r="T384">
+        <f t="shared" si="15"/>
+        <v>0.17166500000000001</v>
+      </c>
+      <c r="U384">
+        <f t="shared" si="14"/>
+        <v>0.23426500000000003</v>
+      </c>
+      <c r="V384">
+        <f t="shared" si="14"/>
+        <v>0.29686499999999999</v>
+      </c>
+    </row>
+    <row r="385" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>498</v>
       </c>
@@ -15267,8 +15369,33 @@
       <c r="L385" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="386" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="P385" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q385">
+        <v>-4.7000000000000002E-3</v>
+      </c>
+      <c r="R385">
+        <v>5.4359999999999999E-2</v>
+      </c>
+      <c r="S385">
+        <f>$Q385-($R385*S$381)</f>
+        <v>-4.5470000000000003E-2</v>
+      </c>
+      <c r="T385">
+        <f>$Q385-($R385*T$381)</f>
+        <v>-5.9060000000000001E-2</v>
+      </c>
+      <c r="U385">
+        <f t="shared" ref="U385:V385" si="16">$Q385-($R385*U$381)</f>
+        <v>-8.6239999999999997E-2</v>
+      </c>
+      <c r="V385">
+        <f t="shared" si="16"/>
+        <v>-0.11341999999999999</v>
+      </c>
+    </row>
+    <row r="386" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>3</v>
       </c>
@@ -15308,7 +15435,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="387" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>5</v>
       </c>
@@ -15348,7 +15475,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="388" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>10</v>
       </c>
@@ -15388,7 +15515,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="389" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>11</v>
       </c>
@@ -15428,7 +15555,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="390" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>13</v>
       </c>
@@ -15468,7 +15595,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="391" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>19</v>
       </c>
@@ -15508,7 +15635,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="392" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>35</v>
       </c>
@@ -15548,7 +15675,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="393" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>40</v>
       </c>
@@ -15588,7 +15715,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="394" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>46</v>
       </c>
@@ -15628,7 +15755,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="395" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>68</v>
       </c>
@@ -15668,7 +15795,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="396" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>85</v>
       </c>
@@ -15708,7 +15835,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="397" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A397">
         <v>91</v>
       </c>
@@ -15748,7 +15875,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="398" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A398">
         <v>101</v>
       </c>
@@ -15788,7 +15915,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="399" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>104</v>
       </c>
@@ -15828,7 +15955,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="400" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A400">
         <v>111</v>
       </c>
@@ -17148,7 +17275,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="433" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A433">
         <v>460</v>
       </c>
@@ -17188,7 +17315,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="434" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A434">
         <v>468</v>
       </c>
@@ -17228,7 +17355,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="435" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A435">
         <v>487</v>
       </c>
@@ -17268,7 +17395,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="436" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A436">
         <v>488</v>
       </c>
@@ -17308,7 +17435,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="437" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A437">
         <v>490</v>
       </c>
@@ -17348,7 +17475,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="438" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A438">
         <v>495</v>
       </c>
@@ -17362,7 +17489,7 @@
         <v>360.36799999999999</v>
       </c>
       <c r="E438">
-        <f t="shared" ref="E438:E446" si="14">D438/C438</f>
+        <f t="shared" ref="E438:E446" si="17">D438/C438</f>
         <v>0.80554836772768856</v>
       </c>
       <c r="F438">
@@ -17372,7 +17499,7 @@
         <v>2.0146099999999998</v>
       </c>
       <c r="H438">
-        <f t="shared" ref="H438:H446" si="15">C438/F438</f>
+        <f t="shared" ref="H438:H446" si="18">C438/F438</f>
         <v>338.28895306455178</v>
       </c>
       <c r="I438" t="s">
@@ -17388,7 +17515,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="439" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A439">
         <v>504</v>
       </c>
@@ -17402,7 +17529,7 @@
         <v>701.35199999999998</v>
       </c>
       <c r="E439">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.75910464741567552</v>
       </c>
       <c r="F439">
@@ -17412,7 +17539,7 @@
         <v>5.4995799999999999</v>
       </c>
       <c r="H439">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>243.32325236516709</v>
       </c>
       <c r="I439" t="s">
@@ -17428,7 +17555,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="440" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A440">
         <v>505</v>
       </c>
@@ -17442,7 +17569,7 @@
         <v>249.916</v>
       </c>
       <c r="E440">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.87018366722889096</v>
       </c>
       <c r="F440">
@@ -17452,7 +17579,7 @@
         <v>1.1059699999999999</v>
       </c>
       <c r="H440">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>277.85729875844243</v>
       </c>
       <c r="I440" t="s">
@@ -17468,7 +17595,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="441" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A441">
         <v>511</v>
       </c>
@@ -17482,7 +17609,7 @@
         <v>420.24599999999998</v>
       </c>
       <c r="E441">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.69609956701465991</v>
       </c>
       <c r="F441">
@@ -17492,7 +17619,7 @@
         <v>2.8856899999999999</v>
       </c>
       <c r="H441">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>276.31549007106577</v>
       </c>
       <c r="I441" t="s">
@@ -17508,7 +17635,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="442" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A442">
         <v>530</v>
       </c>
@@ -17522,7 +17649,7 @@
         <v>325.71100000000001</v>
       </c>
       <c r="E442">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.82100495623474246</v>
       </c>
       <c r="F442">
@@ -17532,7 +17659,7 @@
         <v>1.88558</v>
       </c>
       <c r="H442">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>237.67142501969499</v>
       </c>
       <c r="I442" t="s">
@@ -17548,7 +17675,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="443" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A443">
         <v>534</v>
       </c>
@@ -17562,7 +17689,7 @@
         <v>296.11500000000001</v>
       </c>
       <c r="E443">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.83696701875095281</v>
       </c>
       <c r="F443">
@@ -17572,7 +17699,7 @@
         <v>1.28085</v>
       </c>
       <c r="H443">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>342.51193241059769</v>
       </c>
       <c r="I443" t="s">
@@ -17588,7 +17715,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="444" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A444">
         <v>540</v>
       </c>
@@ -17602,7 +17729,7 @@
         <v>412.197</v>
       </c>
       <c r="E444">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.79268482504280124</v>
       </c>
       <c r="F444">
@@ -17612,7 +17739,7 @@
         <v>2.7820900000000002</v>
       </c>
       <c r="H444">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>219.41605244369882</v>
       </c>
       <c r="I444" t="s">
@@ -17628,7 +17755,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="445" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A445">
         <v>568</v>
       </c>
@@ -17642,7 +17769,7 @@
         <v>302.68700000000001</v>
       </c>
       <c r="E445">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.78889791406824039</v>
       </c>
       <c r="F445">
@@ -17652,7 +17779,7 @@
         <v>1.5160199999999999</v>
       </c>
       <c r="H445">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>320.72101160647486</v>
       </c>
       <c r="I445" t="s">
@@ -17668,7 +17795,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="446" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A446">
         <v>584</v>
       </c>
@@ -17682,7 +17809,7 @@
         <v>538.64599999999996</v>
       </c>
       <c r="E446">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.77618800242173025</v>
       </c>
       <c r="F446">
@@ -17692,7 +17819,7 @@
         <v>4.0633900000000001</v>
       </c>
       <c r="H446">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>258.80402204201948</v>
       </c>
       <c r="I446" t="s">
@@ -17708,9 +17835,1718 @@
         <v>13</v>
       </c>
     </row>
+    <row r="448" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A448">
+        <v>70</v>
+      </c>
+      <c r="B448" t="s">
+        <v>38</v>
+      </c>
+      <c r="C448">
+        <v>602.921786</v>
+      </c>
+      <c r="D448">
+        <v>486.00299999999999</v>
+      </c>
+      <c r="E448">
+        <f>D448/C448</f>
+        <v>0.80607967946276859</v>
+      </c>
+      <c r="F448">
+        <v>3.7817820000000002</v>
+      </c>
+      <c r="G448">
+        <v>4.2339500000000001</v>
+      </c>
+      <c r="H448">
+        <f>C448/F448</f>
+        <v>159.42795909441634</v>
+      </c>
+      <c r="I448" t="s">
+        <v>4</v>
+      </c>
+      <c r="J448" t="s">
+        <v>4</v>
+      </c>
+      <c r="K448" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q448">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="449" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A449">
+        <v>90</v>
+      </c>
+      <c r="B449" t="s">
+        <v>38</v>
+      </c>
+      <c r="C449">
+        <v>485.94799899999998</v>
+      </c>
+      <c r="D449">
+        <v>400.41199999999998</v>
+      </c>
+      <c r="E449">
+        <f>D449/C449</f>
+        <v>0.82398116840481117</v>
+      </c>
+      <c r="F449">
+        <v>2.732901</v>
+      </c>
+      <c r="G449">
+        <v>2.9589300000000001</v>
+      </c>
+      <c r="H449">
+        <f>C449/F449</f>
+        <v>177.81397825973204</v>
+      </c>
+      <c r="Q449">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="450" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A450">
+        <v>97</v>
+      </c>
+      <c r="B450" t="s">
+        <v>38</v>
+      </c>
+      <c r="C450">
+        <v>581.80897700000003</v>
+      </c>
+      <c r="D450">
+        <v>426.49400000000003</v>
+      </c>
+      <c r="E450">
+        <f>D450/C450</f>
+        <v>0.73304815989458338</v>
+      </c>
+      <c r="F450">
+        <v>1.535709</v>
+      </c>
+      <c r="G450">
+        <v>2.4571299999999998</v>
+      </c>
+      <c r="H450">
+        <f>C450/F450</f>
+        <v>378.85366107771722</v>
+      </c>
+      <c r="Q450">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="451" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A451">
+        <v>105</v>
+      </c>
+      <c r="B451" t="s">
+        <v>38</v>
+      </c>
+      <c r="C451">
+        <v>345.79219799999998</v>
+      </c>
+      <c r="D451">
+        <v>278.48200000000003</v>
+      </c>
+      <c r="E451">
+        <f>D451/C451</f>
+        <v>0.80534494881807606</v>
+      </c>
+      <c r="F451">
+        <v>0.90099899999999999</v>
+      </c>
+      <c r="G451">
+        <v>1.25935</v>
+      </c>
+      <c r="H451">
+        <f>C451/F451</f>
+        <v>383.78754915377266</v>
+      </c>
+      <c r="Q451">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="452" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A452">
+        <v>115</v>
+      </c>
+      <c r="B452" t="s">
+        <v>38</v>
+      </c>
+      <c r="C452">
+        <v>318.59512599999999</v>
+      </c>
+      <c r="D452">
+        <v>262.90100000000001</v>
+      </c>
+      <c r="E452">
+        <f>D452/C452</f>
+        <v>0.82518839286951307</v>
+      </c>
+      <c r="F452">
+        <v>0.90099899999999999</v>
+      </c>
+      <c r="G452">
+        <v>1.0852999999999999</v>
+      </c>
+      <c r="H452">
+        <f>C452/F452</f>
+        <v>353.60208612884145</v>
+      </c>
+      <c r="Q452">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="453" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A453">
+        <v>116</v>
+      </c>
+      <c r="B453" t="s">
+        <v>38</v>
+      </c>
+      <c r="C453">
+        <v>695.14100599999995</v>
+      </c>
+      <c r="D453">
+        <v>508.863</v>
+      </c>
+      <c r="E453">
+        <f>D453/C453</f>
+        <v>0.7320284598489073</v>
+      </c>
+      <c r="F453">
+        <v>2.0067400000000002</v>
+      </c>
+      <c r="G453">
+        <v>3.5629900000000001</v>
+      </c>
+      <c r="H453">
+        <f>C453/F453</f>
+        <v>346.40312447053424</v>
+      </c>
+      <c r="Q453">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="454" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A454">
+        <v>185</v>
+      </c>
+      <c r="B454" t="s">
+        <v>38</v>
+      </c>
+      <c r="C454">
+        <v>797.92326100000002</v>
+      </c>
+      <c r="D454">
+        <v>488.56400000000002</v>
+      </c>
+      <c r="E454">
+        <f>D454/C454</f>
+        <v>0.6122944697560333</v>
+      </c>
+      <c r="F454">
+        <v>2.7039569999999999</v>
+      </c>
+      <c r="G454">
+        <v>3.82036</v>
+      </c>
+      <c r="H454">
+        <f>C454/F454</f>
+        <v>295.09465609105473</v>
+      </c>
+      <c r="Q454">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="455" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A455">
+        <v>272</v>
+      </c>
+      <c r="B455" t="s">
+        <v>38</v>
+      </c>
+      <c r="C455">
+        <v>286.14093200000002</v>
+      </c>
+      <c r="D455">
+        <v>246.81700000000001</v>
+      </c>
+      <c r="E455">
+        <f>D455/C455</f>
+        <v>0.86257145482422626</v>
+      </c>
+      <c r="F455">
+        <v>0.90401699999999996</v>
+      </c>
+      <c r="G455">
+        <v>1.03756</v>
+      </c>
+      <c r="H455">
+        <f>C455/F455</f>
+        <v>316.52162735877761</v>
+      </c>
+      <c r="I455" t="s">
+        <v>4</v>
+      </c>
+      <c r="J455" t="s">
+        <v>4</v>
+      </c>
+      <c r="K455" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q455">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="456" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A456">
+        <v>282</v>
+      </c>
+      <c r="B456" t="s">
+        <v>38</v>
+      </c>
+      <c r="C456">
+        <v>462.74645800000002</v>
+      </c>
+      <c r="D456">
+        <v>338.66399999999999</v>
+      </c>
+      <c r="E456">
+        <f>D456/C456</f>
+        <v>0.73185649321598911</v>
+      </c>
+      <c r="F456">
+        <v>0.86040499999999998</v>
+      </c>
+      <c r="G456">
+        <v>1.57741</v>
+      </c>
+      <c r="H456">
+        <f>C456/F456</f>
+        <v>537.82399916318479</v>
+      </c>
+      <c r="Q456">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="457" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A457">
+        <v>313</v>
+      </c>
+      <c r="B457" t="s">
+        <v>38</v>
+      </c>
+      <c r="C457">
+        <v>546.04580399999998</v>
+      </c>
+      <c r="D457">
+        <v>388.64699999999999</v>
+      </c>
+      <c r="E457">
+        <f>D457/C457</f>
+        <v>0.71174798369112646</v>
+      </c>
+      <c r="F457">
+        <v>1.704847</v>
+      </c>
+      <c r="G457">
+        <v>2.4853800000000001</v>
+      </c>
+      <c r="H457">
+        <f>C457/F457</f>
+        <v>320.29021020654636</v>
+      </c>
+      <c r="Q457">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="458" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A458">
+        <v>327</v>
+      </c>
+      <c r="B458" t="s">
+        <v>38</v>
+      </c>
+      <c r="C458">
+        <v>383.12779399999999</v>
+      </c>
+      <c r="D458">
+        <v>304.94200000000001</v>
+      </c>
+      <c r="E458">
+        <f>D458/C458</f>
+        <v>0.79592763765919838</v>
+      </c>
+      <c r="F458">
+        <v>1.5627679999999999</v>
+      </c>
+      <c r="G458">
+        <v>1.7272700000000001</v>
+      </c>
+      <c r="H458">
+        <f>C458/F458</f>
+        <v>245.1597383616762</v>
+      </c>
+      <c r="Q458">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="459" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A459">
+        <v>349</v>
+      </c>
+      <c r="B459" t="s">
+        <v>38</v>
+      </c>
+      <c r="C459">
+        <v>399.15229199999999</v>
+      </c>
+      <c r="D459">
+        <v>282.46100000000001</v>
+      </c>
+      <c r="E459">
+        <f>D459/C459</f>
+        <v>0.70765220609080215</v>
+      </c>
+      <c r="F459">
+        <v>0.75865800000000005</v>
+      </c>
+      <c r="G459">
+        <v>1.2917700000000001</v>
+      </c>
+      <c r="H459">
+        <f>C459/F459</f>
+        <v>526.12941799862381</v>
+      </c>
+      <c r="Q459">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="460" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A460">
+        <v>362</v>
+      </c>
+      <c r="B460" t="s">
+        <v>38</v>
+      </c>
+      <c r="C460">
+        <v>522.41210799999999</v>
+      </c>
+      <c r="D460">
+        <v>411.95800000000003</v>
+      </c>
+      <c r="E460">
+        <f>D460/C460</f>
+        <v>0.78856901226339882</v>
+      </c>
+      <c r="F460">
+        <v>1.971395</v>
+      </c>
+      <c r="G460">
+        <v>2.64907</v>
+      </c>
+      <c r="H460">
+        <f>C460/F460</f>
+        <v>264.99616160130262</v>
+      </c>
+      <c r="Q460">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="461" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A461">
+        <v>386</v>
+      </c>
+      <c r="B461" t="s">
+        <v>38</v>
+      </c>
+      <c r="C461">
+        <v>410.17359199999999</v>
+      </c>
+      <c r="D461">
+        <v>311.95499999999998</v>
+      </c>
+      <c r="E461">
+        <f>D461/C461</f>
+        <v>0.76054384310533574</v>
+      </c>
+      <c r="F461">
+        <v>0.98724999999999996</v>
+      </c>
+      <c r="G461">
+        <v>1.43974</v>
+      </c>
+      <c r="H461">
+        <f>C461/F461</f>
+        <v>415.47084527728538</v>
+      </c>
+      <c r="Q461">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="462" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A462">
+        <v>418</v>
+      </c>
+      <c r="B462" t="s">
+        <v>38</v>
+      </c>
+      <c r="C462">
+        <v>547.90136500000006</v>
+      </c>
+      <c r="D462">
+        <v>520.255</v>
+      </c>
+      <c r="E462">
+        <f>D462/C462</f>
+        <v>0.94954134673491819</v>
+      </c>
+      <c r="F462">
+        <v>1.4809969999999999</v>
+      </c>
+      <c r="G462">
+        <v>1.7175499999999999</v>
+      </c>
+      <c r="H462">
+        <f>C462/F462</f>
+        <v>369.95440571452883</v>
+      </c>
+      <c r="I462" t="s">
+        <v>3</v>
+      </c>
+      <c r="J462" t="s">
+        <v>3</v>
+      </c>
+      <c r="K462" t="s">
+        <v>3</v>
+      </c>
+      <c r="L462" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q462">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="463" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A463">
+        <v>419</v>
+      </c>
+      <c r="B463" t="s">
+        <v>38</v>
+      </c>
+      <c r="C463">
+        <v>436.19800400000003</v>
+      </c>
+      <c r="D463">
+        <v>348.50400000000002</v>
+      </c>
+      <c r="E463">
+        <f>D463/C463</f>
+        <v>0.7989582639172278</v>
+      </c>
+      <c r="F463">
+        <v>1.49987</v>
+      </c>
+      <c r="G463">
+        <v>1.80806</v>
+      </c>
+      <c r="H463">
+        <f>C463/F463</f>
+        <v>290.823874069086</v>
+      </c>
+      <c r="Q463">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="464" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A464">
+        <v>432</v>
+      </c>
+      <c r="B464" t="s">
+        <v>38</v>
+      </c>
+      <c r="C464">
+        <v>951.40107699999999</v>
+      </c>
+      <c r="D464">
+        <v>615.26300000000003</v>
+      </c>
+      <c r="E464">
+        <f>D464/C464</f>
+        <v>0.6466915109451784</v>
+      </c>
+      <c r="F464">
+        <v>2.8063760000000002</v>
+      </c>
+      <c r="G464">
+        <v>6.5448000000000004</v>
+      </c>
+      <c r="H464">
+        <f>C464/F464</f>
+        <v>339.01411535731489</v>
+      </c>
+      <c r="Q464">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="465" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A465">
+        <v>473</v>
+      </c>
+      <c r="B465" t="s">
+        <v>38</v>
+      </c>
+      <c r="C465">
+        <v>629.36500100000001</v>
+      </c>
+      <c r="D465">
+        <v>529.59199999999998</v>
+      </c>
+      <c r="E465">
+        <f>D465/C465</f>
+        <v>0.84147036959241395</v>
+      </c>
+      <c r="F465">
+        <v>1.254624</v>
+      </c>
+      <c r="G465">
+        <v>3.5067699999999999</v>
+      </c>
+      <c r="H465">
+        <f>C465/F465</f>
+        <v>501.63634762287347</v>
+      </c>
+      <c r="I465" t="s">
+        <v>3</v>
+      </c>
+      <c r="J465" t="s">
+        <v>3</v>
+      </c>
+      <c r="K465" t="s">
+        <v>3</v>
+      </c>
+      <c r="L465" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q465">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="466" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A466">
+        <v>526</v>
+      </c>
+      <c r="B466" t="s">
+        <v>38</v>
+      </c>
+      <c r="C466">
+        <v>525.55159000000003</v>
+      </c>
+      <c r="D466">
+        <v>395.63099999999997</v>
+      </c>
+      <c r="E466">
+        <f>D466/C466</f>
+        <v>0.75279193808546929</v>
+      </c>
+      <c r="F466">
+        <v>1.1689130000000001</v>
+      </c>
+      <c r="G466">
+        <v>2.3275700000000001</v>
+      </c>
+      <c r="H466">
+        <f>C466/F466</f>
+        <v>449.60710506256669</v>
+      </c>
+      <c r="Q466">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="467" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A467">
+        <v>533</v>
+      </c>
+      <c r="B467" t="s">
+        <v>38</v>
+      </c>
+      <c r="C467">
+        <v>559.74976800000002</v>
+      </c>
+      <c r="D467">
+        <v>384.40800000000002</v>
+      </c>
+      <c r="E467">
+        <f>D467/C467</f>
+        <v>0.68674972635272269</v>
+      </c>
+      <c r="F467">
+        <v>1.3740140000000001</v>
+      </c>
+      <c r="G467">
+        <v>2.3891399999999998</v>
+      </c>
+      <c r="H467">
+        <f>C467/F467</f>
+        <v>407.38287091689023</v>
+      </c>
+      <c r="Q467">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="468" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A468">
+        <v>534</v>
+      </c>
+      <c r="B468" t="s">
+        <v>38</v>
+      </c>
+      <c r="C468">
+        <v>442.852192</v>
+      </c>
+      <c r="D468">
+        <v>339.68700000000001</v>
+      </c>
+      <c r="E468">
+        <f>D468/C468</f>
+        <v>0.76704373634442802</v>
+      </c>
+      <c r="F468">
+        <v>1.4354990000000001</v>
+      </c>
+      <c r="G468">
+        <v>1.8353900000000001</v>
+      </c>
+      <c r="H468">
+        <f>C468/F468</f>
+        <v>308.5005228147146</v>
+      </c>
+      <c r="Q468">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="469" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A469">
+        <v>633</v>
+      </c>
+      <c r="B469" t="s">
+        <v>38</v>
+      </c>
+      <c r="C469">
+        <v>406.10143799999997</v>
+      </c>
+      <c r="D469">
+        <v>302.40300000000002</v>
+      </c>
+      <c r="E469">
+        <f>D469/C469</f>
+        <v>0.74464892685260586</v>
+      </c>
+      <c r="F469">
+        <v>1.1063860000000001</v>
+      </c>
+      <c r="G469">
+        <v>1.36249</v>
+      </c>
+      <c r="H469">
+        <f>C469/F469</f>
+        <v>367.05222047278249</v>
+      </c>
+      <c r="Q469">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="470" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A470">
+        <v>649</v>
+      </c>
+      <c r="B470" t="s">
+        <v>38</v>
+      </c>
+      <c r="C470">
+        <v>450.24839400000002</v>
+      </c>
+      <c r="D470">
+        <v>336.28300000000002</v>
+      </c>
+      <c r="E470">
+        <f>D470/C470</f>
+        <v>0.7468832859401604</v>
+      </c>
+      <c r="F470">
+        <v>1.1513340000000001</v>
+      </c>
+      <c r="G470">
+        <v>1.5419700000000001</v>
+      </c>
+      <c r="H470">
+        <f>C470/F470</f>
+        <v>391.06670523062809</v>
+      </c>
+      <c r="Q470">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="471" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A471">
+        <v>691</v>
+      </c>
+      <c r="B471" t="s">
+        <v>38</v>
+      </c>
+      <c r="C471">
+        <v>842.30425700000001</v>
+      </c>
+      <c r="D471">
+        <v>519.03</v>
+      </c>
+      <c r="E471">
+        <f>D471/C471</f>
+        <v>0.61620251314959218</v>
+      </c>
+      <c r="F471">
+        <v>3.5988319999999998</v>
+      </c>
+      <c r="G471">
+        <v>4.4419899999999997</v>
+      </c>
+      <c r="H471">
+        <f>C471/F471</f>
+        <v>234.04934073054815</v>
+      </c>
+      <c r="I471" t="s">
+        <v>4</v>
+      </c>
+      <c r="J471" t="s">
+        <v>4</v>
+      </c>
+      <c r="K471" t="s">
+        <v>4</v>
+      </c>
+      <c r="L471" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q471">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="472" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A472">
+        <v>702</v>
+      </c>
+      <c r="B472" t="s">
+        <v>38</v>
+      </c>
+      <c r="C472">
+        <v>526.30000299999995</v>
+      </c>
+      <c r="D472">
+        <v>355.91</v>
+      </c>
+      <c r="E472">
+        <f>D472/C472</f>
+        <v>0.67624928362388792</v>
+      </c>
+      <c r="F472">
+        <v>1.1927779999999999</v>
+      </c>
+      <c r="G472">
+        <v>2.0565199999999999</v>
+      </c>
+      <c r="H472">
+        <f>C472/F472</f>
+        <v>441.23885836257875</v>
+      </c>
+      <c r="I472" t="s">
+        <v>4</v>
+      </c>
+      <c r="J472" t="s">
+        <v>4</v>
+      </c>
+      <c r="K472" t="s">
+        <v>4</v>
+      </c>
+      <c r="L472" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q472">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="473" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A473">
+        <v>707</v>
+      </c>
+      <c r="B473" t="s">
+        <v>38</v>
+      </c>
+      <c r="C473">
+        <v>746.26001599999995</v>
+      </c>
+      <c r="D473">
+        <v>502.03300000000002</v>
+      </c>
+      <c r="E473">
+        <f>D473/C473</f>
+        <v>0.67273200926793331</v>
+      </c>
+      <c r="F473">
+        <v>2.4679980000000001</v>
+      </c>
+      <c r="G473">
+        <v>4.07219</v>
+      </c>
+      <c r="H473">
+        <f>C473/F473</f>
+        <v>302.37464373958159</v>
+      </c>
+      <c r="I473" t="s">
+        <v>4</v>
+      </c>
+      <c r="J473" t="s">
+        <v>4</v>
+      </c>
+      <c r="K473" t="s">
+        <v>4</v>
+      </c>
+      <c r="L473" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q473">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="474" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A474">
+        <v>710</v>
+      </c>
+      <c r="B474" t="s">
+        <v>38</v>
+      </c>
+      <c r="C474">
+        <v>513.20097399999997</v>
+      </c>
+      <c r="D474">
+        <v>365.49099999999999</v>
+      </c>
+      <c r="E474">
+        <f>D474/C474</f>
+        <v>0.71217908483548586</v>
+      </c>
+      <c r="F474">
+        <v>1.234024</v>
+      </c>
+      <c r="G474">
+        <v>2.0772699999999999</v>
+      </c>
+      <c r="H474">
+        <f>C474/F474</f>
+        <v>415.87600727376451</v>
+      </c>
+      <c r="I474" t="s">
+        <v>4</v>
+      </c>
+      <c r="J474" t="s">
+        <v>4</v>
+      </c>
+      <c r="K474" t="s">
+        <v>4</v>
+      </c>
+      <c r="L474" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q474">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="475" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A475">
+        <v>711</v>
+      </c>
+      <c r="B475" t="s">
+        <v>38</v>
+      </c>
+      <c r="C475">
+        <v>296.72134799999998</v>
+      </c>
+      <c r="D475">
+        <v>245.52699999999999</v>
+      </c>
+      <c r="E475">
+        <f>D475/C475</f>
+        <v>0.82746658322676536</v>
+      </c>
+      <c r="F475">
+        <v>0.90489900000000001</v>
+      </c>
+      <c r="G475">
+        <v>1.0385800000000001</v>
+      </c>
+      <c r="H475">
+        <f>C475/F475</f>
+        <v>327.90548779477047</v>
+      </c>
+      <c r="I475" t="s">
+        <v>4</v>
+      </c>
+      <c r="J475" t="s">
+        <v>4</v>
+      </c>
+      <c r="K475" t="s">
+        <v>4</v>
+      </c>
+      <c r="L475" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q475">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="476" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A476">
+        <v>727</v>
+      </c>
+      <c r="B476" t="s">
+        <v>38</v>
+      </c>
+      <c r="C476">
+        <v>366.56658499999998</v>
+      </c>
+      <c r="D476">
+        <v>275.20600000000002</v>
+      </c>
+      <c r="E476">
+        <f>D476/C476</f>
+        <v>0.7507667399634913</v>
+      </c>
+      <c r="F476">
+        <v>0.88435299999999994</v>
+      </c>
+      <c r="G476">
+        <v>1.20313</v>
+      </c>
+      <c r="H476">
+        <f>C476/F476</f>
+        <v>414.50256289061042</v>
+      </c>
+      <c r="I476" t="s">
+        <v>4</v>
+      </c>
+      <c r="J476" t="s">
+        <v>4</v>
+      </c>
+      <c r="K476" t="s">
+        <v>4</v>
+      </c>
+      <c r="L476" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q476">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="477" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A477">
+        <v>729</v>
+      </c>
+      <c r="B477" t="s">
+        <v>38</v>
+      </c>
+      <c r="C477">
+        <v>376.204815</v>
+      </c>
+      <c r="D477">
+        <v>300.80799999999999</v>
+      </c>
+      <c r="E477">
+        <f>D477/C477</f>
+        <v>0.79958572566382491</v>
+      </c>
+      <c r="F477">
+        <v>1.3161670000000001</v>
+      </c>
+      <c r="G477">
+        <v>1.5629500000000001</v>
+      </c>
+      <c r="H477">
+        <f>C477/F477</f>
+        <v>285.83364800971304</v>
+      </c>
+      <c r="I477" t="s">
+        <v>4</v>
+      </c>
+      <c r="J477" t="s">
+        <v>4</v>
+      </c>
+      <c r="K477" t="s">
+        <v>4</v>
+      </c>
+      <c r="L477" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q477">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="478" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A478">
+        <v>735</v>
+      </c>
+      <c r="B478" t="s">
+        <v>38</v>
+      </c>
+      <c r="C478">
+        <v>353.43855100000002</v>
+      </c>
+      <c r="D478">
+        <v>287.05500000000001</v>
+      </c>
+      <c r="E478">
+        <f>D478/C478</f>
+        <v>0.8121779562184771</v>
+      </c>
+      <c r="F478">
+        <v>1.0077039999999999</v>
+      </c>
+      <c r="G478">
+        <v>1.29562</v>
+      </c>
+      <c r="H478">
+        <f>C478/F478</f>
+        <v>350.7364771798068</v>
+      </c>
+      <c r="I478" t="s">
+        <v>4</v>
+      </c>
+      <c r="J478" t="s">
+        <v>4</v>
+      </c>
+      <c r="K478" t="s">
+        <v>4</v>
+      </c>
+      <c r="L478" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q478">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="479" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A479">
+        <v>737</v>
+      </c>
+      <c r="B479" t="s">
+        <v>38</v>
+      </c>
+      <c r="C479">
+        <v>832.64245600000004</v>
+      </c>
+      <c r="D479">
+        <v>531.20699999999999</v>
+      </c>
+      <c r="E479">
+        <f>D479/C479</f>
+        <v>0.63797731688089654</v>
+      </c>
+      <c r="F479">
+        <v>2.7144599999999999</v>
+      </c>
+      <c r="G479">
+        <v>4.3801500000000004</v>
+      </c>
+      <c r="H479">
+        <f>C479/F479</f>
+        <v>306.74331395563024</v>
+      </c>
+      <c r="I479" t="s">
+        <v>4</v>
+      </c>
+      <c r="J479" t="s">
+        <v>4</v>
+      </c>
+      <c r="K479" t="s">
+        <v>4</v>
+      </c>
+      <c r="L479" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q479">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="480" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A480">
+        <v>744</v>
+      </c>
+      <c r="B480" t="s">
+        <v>38</v>
+      </c>
+      <c r="C480">
+        <v>502.77228300000002</v>
+      </c>
+      <c r="D480">
+        <v>370.06400000000002</v>
+      </c>
+      <c r="E480">
+        <f>D480/C480</f>
+        <v>0.73604693916669228</v>
+      </c>
+      <c r="F480">
+        <v>1.7275210000000001</v>
+      </c>
+      <c r="G480">
+        <v>2.2313800000000001</v>
+      </c>
+      <c r="H480">
+        <f>C480/F480</f>
+        <v>291.03685743907022</v>
+      </c>
+      <c r="I480" t="s">
+        <v>4</v>
+      </c>
+      <c r="J480" t="s">
+        <v>4</v>
+      </c>
+      <c r="K480" t="s">
+        <v>4</v>
+      </c>
+      <c r="L480" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q480">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="481" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A481">
+        <v>747</v>
+      </c>
+      <c r="B481" t="s">
+        <v>38</v>
+      </c>
+      <c r="C481">
+        <v>768.98803899999996</v>
+      </c>
+      <c r="D481">
+        <v>530.029</v>
+      </c>
+      <c r="E481">
+        <f>D481/C481</f>
+        <v>0.68925519399398616</v>
+      </c>
+      <c r="F481">
+        <v>2.118144</v>
+      </c>
+      <c r="G481">
+        <v>3.7941600000000002</v>
+      </c>
+      <c r="H481">
+        <f>C481/F481</f>
+        <v>363.04804536424336</v>
+      </c>
+      <c r="I481" t="s">
+        <v>4</v>
+      </c>
+      <c r="J481" t="s">
+        <v>4</v>
+      </c>
+      <c r="K481" t="s">
+        <v>4</v>
+      </c>
+      <c r="L481" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q481">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="482" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A482">
+        <v>750</v>
+      </c>
+      <c r="B482" t="s">
+        <v>38</v>
+      </c>
+      <c r="C482">
+        <v>383.15052700000001</v>
+      </c>
+      <c r="D482">
+        <v>300.37400000000002</v>
+      </c>
+      <c r="E482">
+        <f>D482/C482</f>
+        <v>0.78395820658756399</v>
+      </c>
+      <c r="F482">
+        <v>1.0693969999999999</v>
+      </c>
+      <c r="G482">
+        <v>1.46014</v>
+      </c>
+      <c r="H482">
+        <f>C482/F482</f>
+        <v>358.28651754212893</v>
+      </c>
+      <c r="I482" t="s">
+        <v>4</v>
+      </c>
+      <c r="J482" t="s">
+        <v>4</v>
+      </c>
+      <c r="K482" t="s">
+        <v>4</v>
+      </c>
+      <c r="L482" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q482">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="483" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A483">
+        <v>755</v>
+      </c>
+      <c r="B483" t="s">
+        <v>38</v>
+      </c>
+      <c r="C483">
+        <v>583.00837799999999</v>
+      </c>
+      <c r="D483">
+        <v>391.64400000000001</v>
+      </c>
+      <c r="E483">
+        <f>D483/C483</f>
+        <v>0.67176393132381373</v>
+      </c>
+      <c r="F483">
+        <v>1.3983730000000001</v>
+      </c>
+      <c r="G483">
+        <v>2.3751799999999998</v>
+      </c>
+      <c r="H483">
+        <f>C483/F483</f>
+        <v>416.91907523958196</v>
+      </c>
+      <c r="I483" t="s">
+        <v>4</v>
+      </c>
+      <c r="J483" t="s">
+        <v>4</v>
+      </c>
+      <c r="K483" t="s">
+        <v>4</v>
+      </c>
+      <c r="L483" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q483">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="484" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A484">
+        <v>832</v>
+      </c>
+      <c r="B484" t="s">
+        <v>38</v>
+      </c>
+      <c r="C484">
+        <v>402.45658700000001</v>
+      </c>
+      <c r="D484">
+        <v>304.47199999999998</v>
+      </c>
+      <c r="E484">
+        <f>D484/C484</f>
+        <v>0.75653377242400555</v>
+      </c>
+      <c r="F484">
+        <v>1.126271</v>
+      </c>
+      <c r="G484">
+        <v>1.5051099999999999</v>
+      </c>
+      <c r="H484">
+        <f>C484/F484</f>
+        <v>357.33547876132832</v>
+      </c>
+      <c r="I484" t="s">
+        <v>4</v>
+      </c>
+      <c r="J484" t="s">
+        <v>4</v>
+      </c>
+      <c r="K484" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q484">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="485" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A485">
+        <v>837</v>
+      </c>
+      <c r="B485" t="s">
+        <v>38</v>
+      </c>
+      <c r="C485">
+        <v>379.64698299999998</v>
+      </c>
+      <c r="D485">
+        <v>309.471</v>
+      </c>
+      <c r="E485">
+        <f>D485/C485</f>
+        <v>0.81515464064678222</v>
+      </c>
+      <c r="F485">
+        <v>1.4187829999999999</v>
+      </c>
+      <c r="G485">
+        <v>1.6552500000000001</v>
+      </c>
+      <c r="H485">
+        <f>C485/F485</f>
+        <v>267.58636310133403</v>
+      </c>
+      <c r="Q485">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="486" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A486">
+        <v>839</v>
+      </c>
+      <c r="B486" t="s">
+        <v>38</v>
+      </c>
+      <c r="C486">
+        <v>620.67974200000003</v>
+      </c>
+      <c r="D486">
+        <v>450.53300000000002</v>
+      </c>
+      <c r="E486">
+        <f>D486/C486</f>
+        <v>0.72587031525833168</v>
+      </c>
+      <c r="F486">
+        <v>1.597235</v>
+      </c>
+      <c r="G486">
+        <v>2.73373</v>
+      </c>
+      <c r="H486">
+        <f>C486/F486</f>
+        <v>388.59638187242331</v>
+      </c>
+      <c r="I486" t="s">
+        <v>4</v>
+      </c>
+      <c r="J486" t="s">
+        <v>4</v>
+      </c>
+      <c r="K486" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q486">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="487" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A487">
+        <v>852</v>
+      </c>
+      <c r="B487" t="s">
+        <v>38</v>
+      </c>
+      <c r="C487">
+        <v>546.53265999999996</v>
+      </c>
+      <c r="D487">
+        <v>459.56</v>
+      </c>
+      <c r="E487">
+        <f>D487/C487</f>
+        <v>0.84086466122628434</v>
+      </c>
+      <c r="F487">
+        <v>2.211538</v>
+      </c>
+      <c r="G487">
+        <v>2.6108500000000001</v>
+      </c>
+      <c r="H487">
+        <f>C487/F487</f>
+        <v>247.1278630527714</v>
+      </c>
+      <c r="I487" t="s">
+        <v>4</v>
+      </c>
+      <c r="J487" t="s">
+        <v>4</v>
+      </c>
+      <c r="K487" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q487">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="488" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A488">
+        <v>865</v>
+      </c>
+      <c r="B488" t="s">
+        <v>38</v>
+      </c>
+      <c r="C488">
+        <v>359.57637899999997</v>
+      </c>
+      <c r="D488">
+        <v>287.83300000000003</v>
+      </c>
+      <c r="E488">
+        <f>D488/C488</f>
+        <v>0.8004780536487911</v>
+      </c>
+      <c r="F488">
+        <v>1.130879</v>
+      </c>
+      <c r="G488">
+        <v>1.3570500000000001</v>
+      </c>
+      <c r="H488">
+        <f>C488/F488</f>
+        <v>317.96185002993246</v>
+      </c>
+      <c r="Q488">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="489" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A489">
+        <v>867</v>
+      </c>
+      <c r="B489" t="s">
+        <v>38</v>
+      </c>
+      <c r="C489">
+        <v>455.55929400000002</v>
+      </c>
+      <c r="D489">
+        <v>345.06299999999999</v>
+      </c>
+      <c r="E489">
+        <f>D489/C489</f>
+        <v>0.75744914996729262</v>
+      </c>
+      <c r="F489">
+        <v>1.433457</v>
+      </c>
+      <c r="G489">
+        <v>1.8123</v>
+      </c>
+      <c r="H489">
+        <f>C489/F489</f>
+        <v>317.80464569219725</v>
+      </c>
+      <c r="I489" t="s">
+        <v>4</v>
+      </c>
+      <c r="J489" t="s">
+        <v>4</v>
+      </c>
+      <c r="K489" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q489">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="490" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A490">
+        <v>885</v>
+      </c>
+      <c r="B490" t="s">
+        <v>38</v>
+      </c>
+      <c r="C490">
+        <v>808.57137</v>
+      </c>
+      <c r="D490">
+        <v>561.82399999999996</v>
+      </c>
+      <c r="E490">
+        <f>D490/C490</f>
+        <v>0.69483538602164452</v>
+      </c>
+      <c r="F490">
+        <v>3.4412509999999998</v>
+      </c>
+      <c r="G490">
+        <v>4.80342</v>
+      </c>
+      <c r="H490">
+        <f>C490/F490</f>
+        <v>234.96436906229741</v>
+      </c>
+      <c r="Q490">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="491" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A491">
+        <v>910</v>
+      </c>
+      <c r="B491" t="s">
+        <v>38</v>
+      </c>
+      <c r="C491">
+        <v>415.48599999999999</v>
+      </c>
+      <c r="D491">
+        <v>308.06</v>
+      </c>
+      <c r="E491">
+        <f>D491/C491</f>
+        <v>0.7414449584342192</v>
+      </c>
+      <c r="F491">
+        <v>0.92182500000000001</v>
+      </c>
+      <c r="G491">
+        <v>1.5056499999999999</v>
+      </c>
+      <c r="H491">
+        <f>C491/F491</f>
+        <v>450.72112385756515</v>
+      </c>
+      <c r="Q491">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="492" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A492">
+        <v>931</v>
+      </c>
+      <c r="B492" t="s">
+        <v>38</v>
+      </c>
+      <c r="C492">
+        <v>289.78488599999997</v>
+      </c>
+      <c r="D492">
+        <v>233.88900000000001</v>
+      </c>
+      <c r="E492">
+        <f>D492/C492</f>
+        <v>0.80711248688104464</v>
+      </c>
+      <c r="F492">
+        <v>0.78153399999999995</v>
+      </c>
+      <c r="G492">
+        <v>0.94606699999999999</v>
+      </c>
+      <c r="H492">
+        <f>C492/F492</f>
+        <v>370.78986454843931</v>
+      </c>
+      <c r="Q492">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="493" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A493">
+        <v>1000</v>
+      </c>
+      <c r="B493" t="s">
+        <v>38</v>
+      </c>
+      <c r="C493">
+        <v>359.52940000000001</v>
+      </c>
+      <c r="D493">
+        <v>296.50299999999999</v>
+      </c>
+      <c r="E493">
+        <f>D493/C493</f>
+        <v>0.82469750735266711</v>
+      </c>
+      <c r="F493">
+        <v>1.0483880000000001</v>
+      </c>
+      <c r="G493">
+        <v>1.3361799999999999</v>
+      </c>
+      <c r="H493">
+        <f>C493/F493</f>
+        <v>342.93543993254406</v>
+      </c>
+      <c r="I493" t="s">
+        <v>4</v>
+      </c>
+      <c r="J493" t="s">
+        <v>4</v>
+      </c>
+      <c r="K493" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q493">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="494" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A494">
+        <v>1007</v>
+      </c>
+      <c r="B494" t="s">
+        <v>38</v>
+      </c>
+      <c r="C494">
+        <v>453.714922</v>
+      </c>
+      <c r="D494">
+        <v>374.12599999999998</v>
+      </c>
+      <c r="E494">
+        <f>D494/C494</f>
+        <v>0.8245838562038742</v>
+      </c>
+      <c r="F494">
+        <v>1.068986</v>
+      </c>
+      <c r="G494">
+        <v>1.60348</v>
+      </c>
+      <c r="H494">
+        <f>C494/F494</f>
+        <v>424.43485882883408</v>
+      </c>
+      <c r="I494" t="s">
+        <v>4</v>
+      </c>
+      <c r="J494" t="s">
+        <v>4</v>
+      </c>
+      <c r="K494" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q494">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:L232">
-    <sortCondition ref="A2:A232"/>
+  <sortState ref="A448:Q494">
+    <sortCondition ref="A448:A494"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>